<commit_message>
Setup for Excel load/save
</commit_message>
<xml_diff>
--- a/Test/KeynoteText.xlsx
+++ b/Test/KeynoteText.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Emacs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="150" windowWidth="23250" windowHeight="12465"/>
+    <workbookView xWindow="11060" yWindow="3540" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="2015.XXX  Keynotes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2856,11 +2856,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -2868,33 +2868,33 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2985,23 +2985,23 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3825,7 +3825,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3860,7 +3860,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4071,18 +4071,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A485" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A475" sqref="A475:XFD475"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="2" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="102.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2">
         <v>0</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4218,22 +4218,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+    <row r="18" spans="1:3" ht="61" customHeight="1">
+      <c r="A18" s="17" t="s">
         <v>739</v>
       </c>
-      <c r="B18" s="20"/>
-    </row>
-    <row r="19" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="18"/>
+    </row>
+    <row r="19" spans="1:3" ht="20" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
     </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="18">
       <c r="A20" s="12" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="42" outlineLevel="1">
       <c r="A21" s="13" t="s">
         <v>560</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="42" outlineLevel="1">
       <c r="A22" s="13" t="s">
         <v>583</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="42" outlineLevel="1">
       <c r="A23" s="13" t="s">
         <v>586</v>
       </c>
@@ -4266,19 +4266,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" outlineLevel="1">
       <c r="A24" s="13"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" outlineLevel="1">
       <c r="A25" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="42" outlineLevel="1">
       <c r="A26" s="6" t="s">
         <v>198</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" outlineLevel="1">
       <c r="A27" s="6" t="s">
         <v>572</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" outlineLevel="1">
       <c r="A28" s="6" t="s">
         <v>578</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="28" outlineLevel="1">
       <c r="A29" s="6" t="s">
         <v>582</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" outlineLevel="1">
       <c r="A30" s="6" t="s">
         <v>595</v>
       </c>
@@ -4333,19 +4333,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" outlineLevel="1">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" outlineLevel="1">
       <c r="A32" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
     </row>
-    <row r="33" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" outlineLevel="1">
       <c r="A33" s="14" t="s">
         <v>196</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="28" outlineLevel="1">
       <c r="A34" s="14" t="s">
         <v>197</v>
       </c>
@@ -4367,24 +4367,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" outlineLevel="1">
       <c r="A35" s="14"/>
       <c r="B35" s="7"/>
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="18">
       <c r="A37" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" outlineLevel="1">
       <c r="A38" s="13" t="s">
         <v>591</v>
       </c>
@@ -4393,19 +4393,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" outlineLevel="1">
       <c r="A39" s="13"/>
       <c r="B39" s="10"/>
       <c r="C39" s="9"/>
     </row>
-    <row r="40" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" outlineLevel="1">
       <c r="A40" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" outlineLevel="1">
       <c r="A41" s="6" t="s">
         <v>200</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" outlineLevel="1">
       <c r="A42" s="6" t="s">
         <v>199</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" outlineLevel="1">
       <c r="A43" s="6" t="s">
         <v>201</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" outlineLevel="1">
       <c r="A44" s="6" t="s">
         <v>202</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" outlineLevel="1">
       <c r="A45" s="6" t="s">
         <v>203</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" outlineLevel="1">
       <c r="A46" s="6" t="s">
         <v>204</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" outlineLevel="1">
       <c r="A47" s="6" t="s">
         <v>205</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" outlineLevel="1">
       <c r="A48" s="6" t="s">
         <v>206</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" outlineLevel="1">
       <c r="A49" s="6" t="s">
         <v>207</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" outlineLevel="1">
       <c r="A50" s="6" t="s">
         <v>208</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" outlineLevel="1">
       <c r="A51" s="6" t="s">
         <v>209</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" outlineLevel="1">
       <c r="A52" s="6" t="s">
         <v>210</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" outlineLevel="1">
       <c r="A53" s="6" t="s">
         <v>211</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" outlineLevel="1">
       <c r="A54" s="6" t="s">
         <v>212</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" outlineLevel="1">
       <c r="A55" s="6" t="s">
         <v>213</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" outlineLevel="1">
       <c r="A56" s="6" t="s">
         <v>214</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" outlineLevel="1">
       <c r="A57" s="6" t="s">
         <v>215</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" outlineLevel="1">
       <c r="A58" s="6" t="s">
         <v>216</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" outlineLevel="1">
       <c r="A59" s="6" t="s">
         <v>217</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" outlineLevel="1">
       <c r="A60" s="6" t="s">
         <v>218</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" outlineLevel="1">
       <c r="A61" s="6" t="s">
         <v>219</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" outlineLevel="1">
       <c r="A62" s="6" t="s">
         <v>220</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" outlineLevel="1">
       <c r="A63" s="6" t="s">
         <v>221</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" outlineLevel="1">
       <c r="A64" s="6" t="s">
         <v>222</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" outlineLevel="1">
       <c r="A65" s="6" t="s">
         <v>223</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" outlineLevel="1">
       <c r="A66" s="6" t="s">
         <v>224</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" outlineLevel="1">
       <c r="A67" s="6" t="s">
         <v>225</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" outlineLevel="1">
       <c r="A68" s="6" t="s">
         <v>226</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" outlineLevel="1">
       <c r="A69" s="6" t="s">
         <v>227</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" outlineLevel="1">
       <c r="A70" s="6" t="s">
         <v>228</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" outlineLevel="1">
       <c r="A71" s="6" t="s">
         <v>229</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" outlineLevel="1">
       <c r="A72" s="6" t="s">
         <v>479</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" outlineLevel="1">
       <c r="A73" s="6" t="s">
         <v>488</v>
       </c>
@@ -4768,19 +4768,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" outlineLevel="1">
       <c r="A74" s="6"/>
       <c r="B74" s="10"/>
       <c r="C74" s="9"/>
     </row>
-    <row r="75" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" outlineLevel="1">
       <c r="A75" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B75" s="16"/>
       <c r="C75" s="16"/>
     </row>
-    <row r="76" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" outlineLevel="1">
       <c r="A76" s="14" t="s">
         <v>230</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" outlineLevel="1">
       <c r="A77" s="14" t="s">
         <v>231</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" outlineLevel="1">
       <c r="A78" s="14" t="s">
         <v>232</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" outlineLevel="1">
       <c r="A79" s="14" t="s">
         <v>233</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" outlineLevel="1">
       <c r="A80" s="14" t="s">
         <v>234</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" outlineLevel="1">
       <c r="A81" s="14" t="s">
         <v>235</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" outlineLevel="1">
       <c r="A82" s="14" t="s">
         <v>236</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="28" outlineLevel="1">
       <c r="A83" s="14" t="s">
         <v>237</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" outlineLevel="1">
       <c r="A84" s="14" t="s">
         <v>238</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" outlineLevel="1">
       <c r="A85" s="14" t="s">
         <v>239</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" outlineLevel="1">
       <c r="A86" s="14" t="s">
         <v>240</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" outlineLevel="1">
       <c r="A87" s="14" t="s">
         <v>241</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" outlineLevel="1">
       <c r="A88" s="14" t="s">
         <v>242</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" outlineLevel="1">
       <c r="A89" s="14" t="s">
         <v>243</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" outlineLevel="1">
       <c r="A90" s="14" t="s">
         <v>244</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" outlineLevel="1">
       <c r="A91" s="14" t="s">
         <v>245</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" outlineLevel="1">
       <c r="A92" s="14" t="s">
         <v>246</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" outlineLevel="1">
       <c r="A93" s="14" t="s">
         <v>247</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" outlineLevel="1">
       <c r="A94" s="14" t="s">
         <v>248</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" outlineLevel="1">
       <c r="A95" s="14" t="s">
         <v>249</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" outlineLevel="1">
       <c r="A96" s="14" t="s">
         <v>250</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" outlineLevel="1">
       <c r="A97" s="14" t="s">
         <v>251</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" outlineLevel="1">
       <c r="A98" s="14" t="s">
         <v>252</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" outlineLevel="1">
       <c r="A99" s="14" t="s">
         <v>253</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" outlineLevel="1">
       <c r="A100" s="14" t="s">
         <v>254</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" outlineLevel="1">
       <c r="A101" s="14" t="s">
         <v>255</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" outlineLevel="1">
       <c r="A102" s="14" t="s">
         <v>256</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" outlineLevel="1">
       <c r="A103" s="14" t="s">
         <v>257</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="28" outlineLevel="1">
       <c r="A104" s="14" t="s">
         <v>258</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="28" outlineLevel="1">
       <c r="A105" s="14" t="s">
         <v>259</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" outlineLevel="1">
       <c r="A106" s="14" t="s">
         <v>260</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="28" outlineLevel="1">
       <c r="A107" s="14" t="s">
         <v>261</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" outlineLevel="1">
       <c r="A108" s="14" t="s">
         <v>262</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" outlineLevel="1">
       <c r="A109" s="14" t="s">
         <v>263</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" outlineLevel="1">
       <c r="A110" s="14" t="s">
         <v>264</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="28" outlineLevel="1">
       <c r="A111" s="14" t="s">
         <v>265</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" outlineLevel="1">
       <c r="A112" s="14" t="s">
         <v>266</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="28" outlineLevel="1">
       <c r="A113" s="14" t="s">
         <v>267</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="28" outlineLevel="1">
       <c r="A114" s="14" t="s">
         <v>268</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" outlineLevel="1">
       <c r="A115" s="14" t="s">
         <v>269</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="28" outlineLevel="1">
       <c r="A116" s="14" t="s">
         <v>270</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" outlineLevel="1">
       <c r="A117" s="14" t="s">
         <v>271</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" outlineLevel="1">
       <c r="A118" s="14" t="s">
         <v>272</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" outlineLevel="1">
       <c r="A119" s="14" t="s">
         <v>273</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" outlineLevel="1">
       <c r="A120" s="14" t="s">
         <v>274</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" outlineLevel="1">
       <c r="A121" s="14" t="s">
         <v>275</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" outlineLevel="1">
       <c r="A122" s="14" t="s">
         <v>276</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" outlineLevel="1">
       <c r="A123" s="14" t="s">
         <v>277</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" outlineLevel="1">
       <c r="A124" s="14" t="s">
         <v>278</v>
       </c>
@@ -5319,24 +5319,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" outlineLevel="1">
       <c r="A125" s="14"/>
       <c r="B125" s="10"/>
       <c r="C125" s="9"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B126" s="16"/>
       <c r="C126" s="16"/>
     </row>
-    <row r="127" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="18">
       <c r="A127" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" outlineLevel="1">
       <c r="A128" s="13" t="s">
         <v>738</v>
       </c>
@@ -5347,19 +5347,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" outlineLevel="1">
       <c r="A129" s="13"/>
       <c r="B129" s="7"/>
       <c r="C129" s="9"/>
     </row>
-    <row r="130" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" outlineLevel="1">
       <c r="A130" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B130" s="16"/>
       <c r="C130" s="16"/>
     </row>
-    <row r="131" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" outlineLevel="1">
       <c r="A131" s="6" t="s">
         <v>489</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" outlineLevel="1">
       <c r="A132" s="6" t="s">
         <v>490</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="28" outlineLevel="1">
       <c r="A133" s="6" t="s">
         <v>491</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="42" outlineLevel="1">
       <c r="A134" s="6" t="s">
         <v>492</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="56" outlineLevel="1">
       <c r="A135" s="6" t="s">
         <v>493</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="42" outlineLevel="1">
       <c r="A136" s="6" t="s">
         <v>494</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="42" outlineLevel="1">
       <c r="A137" s="6" t="s">
         <v>495</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="28" outlineLevel="1">
       <c r="A138" s="6" t="s">
         <v>496</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="28" outlineLevel="1">
       <c r="A139" s="6" t="s">
         <v>692</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="28" outlineLevel="1">
       <c r="A140" s="6" t="s">
         <v>694</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="28" outlineLevel="1">
       <c r="A141" s="6" t="s">
         <v>696</v>
       </c>
@@ -5480,19 +5480,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" outlineLevel="1">
       <c r="A142" s="6"/>
       <c r="B142" s="7"/>
       <c r="C142" s="9"/>
     </row>
-    <row r="143" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" outlineLevel="1">
       <c r="A143" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B143" s="16"/>
       <c r="C143" s="16"/>
     </row>
-    <row r="144" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" outlineLevel="1">
       <c r="A144" s="14" t="s">
         <v>737</v>
       </c>
@@ -5503,24 +5503,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" outlineLevel="1">
       <c r="A145" s="14"/>
       <c r="B145" s="7"/>
       <c r="C145" s="8"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="A146" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B146" s="16"/>
       <c r="C146" s="16"/>
     </row>
-    <row r="147" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="18">
       <c r="A147" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="3" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" s="3" customFormat="1" ht="56" outlineLevel="1">
       <c r="A148" s="13" t="s">
         <v>279</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="56" outlineLevel="1">
       <c r="A149" s="13" t="s">
         <v>280</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" outlineLevel="1">
       <c r="A150" s="13" t="s">
         <v>281</v>
       </c>
@@ -5553,19 +5553,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" outlineLevel="1">
       <c r="A151" s="13"/>
       <c r="B151" s="7"/>
       <c r="C151" s="9"/>
     </row>
-    <row r="152" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" outlineLevel="1">
       <c r="A152" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B152" s="16"/>
       <c r="C152" s="16"/>
     </row>
-    <row r="153" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" outlineLevel="1">
       <c r="A153" s="6" t="s">
         <v>282</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="28" outlineLevel="1">
       <c r="A154" s="6" t="s">
         <v>283</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" outlineLevel="1">
       <c r="A155" s="6" t="s">
         <v>284</v>
       </c>
@@ -5598,19 +5598,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" outlineLevel="1">
       <c r="A156" s="6"/>
       <c r="B156" s="7"/>
       <c r="C156" s="9"/>
     </row>
-    <row r="157" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" outlineLevel="1">
       <c r="A157" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B157" s="16"/>
       <c r="C157" s="16"/>
     </row>
-    <row r="158" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" outlineLevel="1">
       <c r="A158" s="14" t="s">
         <v>285</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="150" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="126" outlineLevel="1">
       <c r="A159" s="14" t="s">
         <v>286</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" outlineLevel="1">
       <c r="A160" s="14" t="s">
         <v>287</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" outlineLevel="1">
       <c r="A161" s="14" t="s">
         <v>288</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" outlineLevel="1">
       <c r="A162" s="14" t="s">
         <v>289</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" outlineLevel="1">
       <c r="A163" s="14" t="s">
         <v>627</v>
       </c>
@@ -5676,24 +5676,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" outlineLevel="1">
       <c r="A164" s="14"/>
       <c r="B164" s="7"/>
       <c r="C164" s="9"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B165" s="16"/>
       <c r="C165" s="16"/>
     </row>
-    <row r="166" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="18">
       <c r="A166" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="28" outlineLevel="2">
       <c r="A167" s="13" t="s">
         <v>290</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="42" outlineLevel="2">
       <c r="A168" s="13" t="s">
         <v>291</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="75" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="56" outlineLevel="2">
       <c r="A169" s="13" t="s">
         <v>292</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="60" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="42" outlineLevel="2">
       <c r="A170" s="13" t="s">
         <v>293</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" outlineLevel="2">
       <c r="A171" s="13" t="s">
         <v>294</v>
       </c>
@@ -5748,33 +5748,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" outlineLevel="2">
       <c r="A172" s="13" t="s">
         <v>295</v>
       </c>
       <c r="B172" s="7"/>
       <c r="C172" s="9"/>
     </row>
-    <row r="173" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" outlineLevel="2">
       <c r="A173" s="13" t="s">
         <v>296</v>
       </c>
       <c r="B173" s="7"/>
       <c r="C173" s="9"/>
     </row>
-    <row r="174" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" outlineLevel="2">
       <c r="A174" s="13"/>
       <c r="B174" s="7"/>
       <c r="C174" s="9"/>
     </row>
-    <row r="175" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" outlineLevel="2">
       <c r="A175" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B175" s="16"/>
       <c r="C175" s="16"/>
     </row>
-    <row r="176" spans="1:3" ht="60" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="56" outlineLevel="2">
       <c r="A176" s="6" t="s">
         <v>300</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="28" outlineLevel="2">
       <c r="A177" s="6" t="s">
         <v>297</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="42" outlineLevel="2">
       <c r="A178" s="6" t="s">
         <v>298</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" outlineLevel="2">
       <c r="A179" s="6" t="s">
         <v>299</v>
       </c>
@@ -5818,19 +5818,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" outlineLevel="2">
       <c r="A180" s="6"/>
       <c r="B180" s="7"/>
       <c r="C180" s="9"/>
     </row>
-    <row r="181" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" outlineLevel="2">
       <c r="A181" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B181" s="16"/>
       <c r="C181" s="16"/>
     </row>
-    <row r="182" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" outlineLevel="2">
       <c r="A182" s="14" t="s">
         <v>301</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="28" outlineLevel="2">
       <c r="A183" s="14" t="s">
         <v>302</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" outlineLevel="2">
       <c r="A184" s="14" t="s">
         <v>303</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="28" outlineLevel="2">
       <c r="A185" s="14" t="s">
         <v>304</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="28" outlineLevel="2">
       <c r="A186" s="14" t="s">
         <v>305</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="60" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="42" outlineLevel="2">
       <c r="A187" s="14" t="s">
         <v>306</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" outlineLevel="2">
       <c r="A188" s="14" t="s">
         <v>307</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="28" outlineLevel="2">
       <c r="A189" s="14" t="s">
         <v>308</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="60" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="56" outlineLevel="2">
       <c r="A190" s="14" t="s">
         <v>309</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" outlineLevel="2">
       <c r="A191" s="14" t="s">
         <v>310</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" outlineLevel="2">
       <c r="A192" s="14" t="s">
         <v>311</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" outlineLevel="2">
       <c r="A193" s="14" t="s">
         <v>312</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" outlineLevel="2">
       <c r="A194" s="14" t="s">
         <v>313</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" outlineLevel="2">
       <c r="A195" s="14" t="s">
         <v>314</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" outlineLevel="2">
       <c r="A196" s="14" t="s">
         <v>315</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" outlineLevel="2">
       <c r="A197" s="14" t="s">
         <v>316</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="28" outlineLevel="2">
       <c r="A198" s="14" t="s">
         <v>317</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="42" outlineLevel="2">
       <c r="A199" s="14" t="s">
         <v>318</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" outlineLevel="2">
       <c r="A200" s="14" t="s">
         <v>682</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" outlineLevel="2">
       <c r="A201" s="14" t="s">
         <v>684</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="28" outlineLevel="2">
       <c r="A202" s="14" t="s">
         <v>702</v>
       </c>
@@ -6061,24 +6061,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" outlineLevel="2">
       <c r="A203" s="14"/>
       <c r="B203" s="7"/>
       <c r="C203" s="9"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3">
       <c r="A204" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B204" s="16"/>
       <c r="C204" s="16"/>
     </row>
-    <row r="205" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="18">
       <c r="A205" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="28" outlineLevel="1">
       <c r="A206" s="13" t="s">
         <v>319</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="42" outlineLevel="1">
       <c r="A207" s="13" t="s">
         <v>320</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="28" outlineLevel="1">
       <c r="A208" s="13" t="s">
         <v>321</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" outlineLevel="1">
       <c r="A209" s="13" t="s">
         <v>322</v>
       </c>
@@ -6122,26 +6122,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" outlineLevel="1">
       <c r="A210" s="13" t="s">
         <v>323</v>
       </c>
       <c r="B210" s="7"/>
       <c r="C210" s="9"/>
     </row>
-    <row r="211" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" outlineLevel="1">
       <c r="A211" s="13"/>
       <c r="B211" s="7"/>
       <c r="C211" s="9"/>
     </row>
-    <row r="212" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" outlineLevel="1">
       <c r="A212" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B212" s="16"/>
       <c r="C212" s="16"/>
     </row>
-    <row r="213" spans="1:3" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="56" outlineLevel="1">
       <c r="A213" s="6" t="s">
         <v>324</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="28" outlineLevel="1">
       <c r="A214" s="6" t="s">
         <v>325</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" outlineLevel="1">
       <c r="A215" s="6" t="s">
         <v>326</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" outlineLevel="1">
       <c r="A216" s="6" t="s">
         <v>327</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" outlineLevel="1">
       <c r="A217" s="6" t="s">
         <v>576</v>
       </c>
@@ -6196,19 +6196,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" outlineLevel="1">
       <c r="A218" s="6"/>
       <c r="B218" s="7"/>
       <c r="C218" s="9"/>
     </row>
-    <row r="219" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" outlineLevel="1">
       <c r="A219" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B219" s="16"/>
       <c r="C219" s="16"/>
     </row>
-    <row r="220" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" outlineLevel="1">
       <c r="A220" s="14" t="s">
         <v>328</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" outlineLevel="1">
       <c r="A221" s="14" t="s">
         <v>329</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" outlineLevel="1">
       <c r="A222" s="14" t="s">
         <v>330</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="28" outlineLevel="1">
       <c r="A223" s="14" t="s">
         <v>331</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" outlineLevel="1">
       <c r="A224" s="14" t="s">
         <v>332</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" outlineLevel="1">
       <c r="A225" s="14" t="s">
         <v>333</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" outlineLevel="1">
       <c r="A226" s="14" t="s">
         <v>334</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" outlineLevel="1">
       <c r="A227" s="14" t="s">
         <v>335</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" outlineLevel="1">
       <c r="A228" s="14" t="s">
         <v>336</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" outlineLevel="1">
       <c r="A229" s="14" t="s">
         <v>337</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" outlineLevel="1">
       <c r="A230" s="14" t="s">
         <v>338</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" outlineLevel="1">
       <c r="A231" s="14" t="s">
         <v>339</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" outlineLevel="1">
       <c r="A232" s="14" t="s">
         <v>340</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="42" outlineLevel="1">
       <c r="A233" s="14" t="s">
         <v>668</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" outlineLevel="1">
       <c r="A234" s="14" t="s">
         <v>675</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="28" outlineLevel="1">
       <c r="A235" s="14" t="s">
         <v>677</v>
       </c>
@@ -6384,24 +6384,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" outlineLevel="1">
       <c r="A236" s="14"/>
       <c r="B236" s="7"/>
       <c r="C236" s="9"/>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3">
       <c r="A237" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B237" s="16"/>
       <c r="C237" s="16"/>
     </row>
-    <row r="238" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" ht="18">
       <c r="A238" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="239" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" outlineLevel="1">
       <c r="A239" s="13" t="s">
         <v>341</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" outlineLevel="1">
       <c r="A240" s="13" t="s">
         <v>342</v>
       </c>
@@ -6423,19 +6423,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" outlineLevel="1">
       <c r="A241" s="13"/>
       <c r="B241" s="7"/>
       <c r="C241" s="9"/>
     </row>
-    <row r="242" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" outlineLevel="1">
       <c r="A242" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B242" s="16"/>
       <c r="C242" s="16"/>
     </row>
-    <row r="243" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="28" outlineLevel="1">
       <c r="A243" s="6" t="s">
         <v>343</v>
       </c>
@@ -6446,19 +6446,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" outlineLevel="1">
       <c r="A244" s="6"/>
       <c r="B244" s="7"/>
       <c r="C244" s="9"/>
     </row>
-    <row r="245" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" outlineLevel="1">
       <c r="A245" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B245" s="16"/>
       <c r="C245" s="16"/>
     </row>
-    <row r="246" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" outlineLevel="1">
       <c r="A246" s="14" t="s">
         <v>344</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" outlineLevel="1">
       <c r="A247" s="14" t="s">
         <v>345</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="28" outlineLevel="1">
       <c r="A248" s="14" t="s">
         <v>346</v>
       </c>
@@ -6491,24 +6491,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" outlineLevel="1">
       <c r="A249" s="14"/>
       <c r="B249" s="7"/>
       <c r="C249" s="9"/>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3">
       <c r="A250" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B250" s="16"/>
       <c r="C250" s="16"/>
     </row>
-    <row r="251" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" ht="18">
       <c r="A251" s="11" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" outlineLevel="1">
       <c r="A252" s="13" t="s">
         <v>347</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" outlineLevel="1">
       <c r="A253" s="13" t="s">
         <v>348</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" ht="28" outlineLevel="1">
       <c r="A254" s="13" t="s">
         <v>349</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="255" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" outlineLevel="1">
       <c r="A255" s="13" t="s">
         <v>350</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="256" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" outlineLevel="1">
       <c r="A256" s="13" t="s">
         <v>701</v>
       </c>
@@ -6563,19 +6563,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="257" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" outlineLevel="1">
       <c r="A257" s="13"/>
       <c r="B257" s="7"/>
       <c r="C257" s="9"/>
     </row>
-    <row r="258" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" outlineLevel="1">
       <c r="A258" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B258" s="16"/>
       <c r="C258" s="16"/>
     </row>
-    <row r="259" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" ht="28" outlineLevel="1">
       <c r="A259" s="6" t="s">
         <v>351</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" outlineLevel="1">
       <c r="A260" s="6" t="s">
         <v>352</v>
       </c>
@@ -6597,19 +6597,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="261" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" outlineLevel="1">
       <c r="A261" s="6"/>
       <c r="B261" s="7"/>
       <c r="C261" s="9"/>
     </row>
-    <row r="262" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" outlineLevel="1">
       <c r="A262" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B262" s="16"/>
       <c r="C262" s="16"/>
     </row>
-    <row r="263" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" ht="42" outlineLevel="1">
       <c r="A263" s="14" t="s">
         <v>353</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" outlineLevel="1">
       <c r="A264" s="14" t="s">
         <v>354</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" ht="28" outlineLevel="1">
       <c r="A265" s="14" t="s">
         <v>355</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" ht="28" outlineLevel="1">
       <c r="A266" s="14" t="s">
         <v>356</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="267" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" outlineLevel="1">
       <c r="A267" s="14" t="s">
         <v>357</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="268" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" outlineLevel="1">
       <c r="A268" s="14" t="s">
         <v>358</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" ht="42" outlineLevel="1">
       <c r="A269" s="14" t="s">
         <v>359</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="270" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" outlineLevel="1">
       <c r="A270" s="14" t="s">
         <v>360</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="271" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" outlineLevel="1">
       <c r="A271" s="14" t="s">
         <v>361</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="272" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" outlineLevel="1">
       <c r="A272" s="14" t="s">
         <v>362</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" ht="28" outlineLevel="1">
       <c r="A273" s="14" t="s">
         <v>363</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="274" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" outlineLevel="1">
       <c r="A274" s="14" t="s">
         <v>364</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" outlineLevel="1">
       <c r="A275" s="14" t="s">
         <v>365</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="276" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" outlineLevel="1">
       <c r="A276" s="14" t="s">
         <v>366</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="277" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" outlineLevel="1">
       <c r="A277" s="14" t="s">
         <v>367</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" ht="28" outlineLevel="1">
       <c r="A278" s="14" t="s">
         <v>368</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" outlineLevel="1">
       <c r="A279" s="14" t="s">
         <v>369</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="280" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" outlineLevel="1">
       <c r="A280" s="14" t="s">
         <v>370</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" ht="56" outlineLevel="1">
       <c r="A281" s="14" t="s">
         <v>371</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" ht="28" outlineLevel="1">
       <c r="A282" s="14" t="s">
         <v>372</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="283" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" outlineLevel="1">
       <c r="A283" s="14" t="s">
         <v>373</v>
       </c>
@@ -6840,24 +6840,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="284" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" outlineLevel="1">
       <c r="A284" s="14"/>
       <c r="B284" s="7"/>
       <c r="C284" s="9"/>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3">
       <c r="A285" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B285" s="16"/>
       <c r="C285" s="16"/>
     </row>
-    <row r="286" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:3" ht="18">
       <c r="A286" s="11" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" outlineLevel="1">
       <c r="A287" s="13" t="s">
         <v>374</v>
       </c>
@@ -6868,19 +6868,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" outlineLevel="1">
       <c r="A288" s="13"/>
       <c r="B288" s="7"/>
       <c r="C288" s="9"/>
     </row>
-    <row r="289" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" outlineLevel="1">
       <c r="A289" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B289" s="16"/>
       <c r="C289" s="16"/>
     </row>
-    <row r="290" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" outlineLevel="1">
       <c r="A290" s="6" t="s">
         <v>376</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" outlineLevel="1">
       <c r="A291" s="6" t="s">
         <v>375</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" outlineLevel="1">
       <c r="A292" s="6" t="s">
         <v>377</v>
       </c>
@@ -6913,19 +6913,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" outlineLevel="1">
       <c r="A293" s="6"/>
       <c r="B293" s="7"/>
       <c r="C293" s="9"/>
     </row>
-    <row r="294" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" outlineLevel="1">
       <c r="A294" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B294" s="16"/>
       <c r="C294" s="16"/>
     </row>
-    <row r="295" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" ht="28" outlineLevel="1">
       <c r="A295" s="14" t="s">
         <v>378</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" outlineLevel="1">
       <c r="A296" s="14" t="s">
         <v>379</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" outlineLevel="1">
       <c r="A297" s="14" t="s">
         <v>380</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" outlineLevel="1">
       <c r="A298" s="14" t="s">
         <v>381</v>
       </c>
@@ -6969,7 +6969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" outlineLevel="1">
       <c r="A299" s="14" t="s">
         <v>382</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" outlineLevel="1">
       <c r="A300" s="14" t="s">
         <v>383</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" ht="28" outlineLevel="1">
       <c r="A301" s="14" t="s">
         <v>384</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="302" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" outlineLevel="1">
       <c r="A302" s="14" t="s">
         <v>385</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="303" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" outlineLevel="1">
       <c r="A303" s="14" t="s">
         <v>386</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="304" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" outlineLevel="1">
       <c r="A304" s="14" t="s">
         <v>387</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="305" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" outlineLevel="1">
       <c r="A305" s="14" t="s">
         <v>388</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="306" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" outlineLevel="1">
       <c r="A306" s="14" t="s">
         <v>389</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="307" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" outlineLevel="1">
       <c r="A307" s="14" t="s">
         <v>390</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="308" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" outlineLevel="1">
       <c r="A308" s="14" t="s">
         <v>391</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="309" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" outlineLevel="1">
       <c r="A309" s="14" t="s">
         <v>392</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="310" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" outlineLevel="1">
       <c r="A310" s="14" t="s">
         <v>393</v>
       </c>
@@ -7101,24 +7101,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="311" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" outlineLevel="1">
       <c r="A311" s="14"/>
       <c r="B311" s="7"/>
       <c r="C311" s="9"/>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3">
       <c r="A312" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B312" s="16"/>
       <c r="C312" s="16"/>
     </row>
-    <row r="313" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:3" ht="18">
       <c r="A313" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="314" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" ht="28" outlineLevel="1">
       <c r="A314" s="13" t="s">
         <v>549</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="315" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" outlineLevel="1">
       <c r="A315" s="13" t="s">
         <v>624</v>
       </c>
@@ -7140,19 +7140,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="316" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" outlineLevel="1">
       <c r="A316" s="13"/>
       <c r="B316" s="7"/>
       <c r="C316" s="9"/>
     </row>
-    <row r="317" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" outlineLevel="1">
       <c r="A317" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B317" s="16"/>
       <c r="C317" s="16"/>
     </row>
-    <row r="318" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" ht="56" outlineLevel="1">
       <c r="A318" s="6" t="s">
         <v>551</v>
       </c>
@@ -7163,19 +7163,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="319" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" outlineLevel="1">
       <c r="A319" s="6"/>
       <c r="B319" s="7"/>
       <c r="C319" s="9"/>
     </row>
-    <row r="320" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" outlineLevel="1">
       <c r="A320" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B320" s="16"/>
       <c r="C320" s="16"/>
     </row>
-    <row r="321" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" outlineLevel="1">
       <c r="A321" s="14" t="s">
         <v>394</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" outlineLevel="1">
       <c r="A322" s="14" t="s">
         <v>395</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" ht="28" outlineLevel="1">
       <c r="A323" s="14" t="s">
         <v>396</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="324" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" outlineLevel="1">
       <c r="A324" s="14" t="s">
         <v>397</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="325" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" ht="28" outlineLevel="1">
       <c r="A325" s="14" t="s">
         <v>398</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="326" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" outlineLevel="1">
       <c r="A326" s="14" t="s">
         <v>399</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="327" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" outlineLevel="1">
       <c r="A327" s="14" t="s">
         <v>400</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="328" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" ht="28" outlineLevel="1">
       <c r="A328" s="14" t="s">
         <v>401</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" ht="28" outlineLevel="1">
       <c r="A329" s="14" t="s">
         <v>402</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="330" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" outlineLevel="1">
       <c r="A330" s="14" t="s">
         <v>403</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="331" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" outlineLevel="1">
       <c r="A331" s="14" t="s">
         <v>404</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="332" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" outlineLevel="1">
       <c r="A332" s="14" t="s">
         <v>405</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="333" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" ht="28" outlineLevel="1">
       <c r="A333" s="14" t="s">
         <v>406</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="334" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" outlineLevel="1">
       <c r="A334" s="14" t="s">
         <v>407</v>
       </c>
@@ -7329,7 +7329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="335" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" outlineLevel="1">
       <c r="A335" s="14" t="s">
         <v>408</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="336" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" ht="28" outlineLevel="1">
       <c r="A336" s="14" t="s">
         <v>409</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="337" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" outlineLevel="1">
       <c r="A337" s="14" t="s">
         <v>410</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="338" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" outlineLevel="1">
       <c r="A338" s="14" t="s">
         <v>505</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="339" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" outlineLevel="1">
       <c r="A339" s="14" t="s">
         <v>506</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="340" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" outlineLevel="1">
       <c r="A340" s="14" t="s">
         <v>507</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="341" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" outlineLevel="1">
       <c r="A341" s="14" t="s">
         <v>511</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="342" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" outlineLevel="1">
       <c r="A342" s="14" t="s">
         <v>513</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="343" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" outlineLevel="1">
       <c r="A343" s="14" t="s">
         <v>673</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" ht="28" outlineLevel="1">
       <c r="A344" s="14" t="s">
         <v>708</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="345" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" outlineLevel="1">
       <c r="A345" s="14" t="s">
         <v>711</v>
       </c>
@@ -7450,24 +7450,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="346" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" outlineLevel="1">
       <c r="A346" s="14"/>
       <c r="B346" s="7"/>
       <c r="C346" s="9"/>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3">
       <c r="A347" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B347" s="16"/>
       <c r="C347" s="16"/>
     </row>
-    <row r="348" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" ht="18">
       <c r="A348" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="349" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" outlineLevel="1">
       <c r="A349" s="13" t="s">
         <v>23</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="350" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" outlineLevel="1">
       <c r="A350" s="13" t="s">
         <v>411</v>
       </c>
@@ -7489,7 +7489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" outlineLevel="1">
       <c r="A351" s="13" t="s">
         <v>412</v>
       </c>
@@ -7500,19 +7500,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="352" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" outlineLevel="1">
       <c r="A352" s="13"/>
       <c r="B352" s="7"/>
       <c r="C352" s="9"/>
     </row>
-    <row r="353" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" outlineLevel="1">
       <c r="A353" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B353" s="16"/>
       <c r="C353" s="16"/>
     </row>
-    <row r="354" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" outlineLevel="1">
       <c r="A354" s="6" t="s">
         <v>735</v>
       </c>
@@ -7523,19 +7523,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="355" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" outlineLevel="1">
       <c r="A355" s="6"/>
       <c r="B355" s="7"/>
       <c r="C355" s="9"/>
     </row>
-    <row r="356" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" outlineLevel="1">
       <c r="A356" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B356" s="16"/>
       <c r="C356" s="16"/>
     </row>
-    <row r="357" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" outlineLevel="1">
       <c r="A357" s="14" t="s">
         <v>451</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="358" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" outlineLevel="1">
       <c r="A358" s="14" t="s">
         <v>452</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="359" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" outlineLevel="1">
       <c r="A359" s="14" t="s">
         <v>453</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="360" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" outlineLevel="1">
       <c r="A360" s="14" t="s">
         <v>454</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" outlineLevel="1">
       <c r="A361" s="14" t="s">
         <v>455</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="362" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" outlineLevel="1">
       <c r="A362" s="14" t="s">
         <v>456</v>
       </c>
@@ -7601,7 +7601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="363" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" outlineLevel="1">
       <c r="A363" s="14" t="s">
         <v>457</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="364" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" outlineLevel="1">
       <c r="A364" s="14" t="s">
         <v>458</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="365" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" ht="28" outlineLevel="1">
       <c r="A365" s="14" t="s">
         <v>459</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="366" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" ht="28" outlineLevel="1">
       <c r="A366" s="14" t="s">
         <v>669</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="367" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" ht="28" outlineLevel="1">
       <c r="A367" s="14" t="s">
         <v>689</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" outlineLevel="1">
       <c r="A368" s="14" t="s">
         <v>691</v>
       </c>
@@ -7667,24 +7667,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" outlineLevel="1">
       <c r="A369" s="14"/>
       <c r="B369" s="7"/>
       <c r="C369" s="9"/>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3">
       <c r="A370" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B370" s="16"/>
       <c r="C370" s="16"/>
     </row>
-    <row r="371" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" ht="18">
       <c r="A371" s="11" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="372" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" outlineLevel="1">
       <c r="A372" s="13" t="s">
         <v>734</v>
       </c>
@@ -7695,19 +7695,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="373" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" outlineLevel="1">
       <c r="A373" s="13"/>
       <c r="B373" s="7"/>
       <c r="C373" s="9"/>
     </row>
-    <row r="374" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" outlineLevel="1">
       <c r="A374" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B374" s="16"/>
       <c r="C374" s="16"/>
     </row>
-    <row r="375" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" outlineLevel="1">
       <c r="A375" s="6" t="s">
         <v>413</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="376" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" outlineLevel="1">
       <c r="A376" s="6" t="s">
         <v>414</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="377" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" outlineLevel="1">
       <c r="A377" s="6" t="s">
         <v>415</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="378" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" outlineLevel="1">
       <c r="A378" s="6" t="s">
         <v>416</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="379" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" outlineLevel="1">
       <c r="A379" s="6" t="s">
         <v>417</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="380" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" outlineLevel="1">
       <c r="A380" s="6" t="s">
         <v>418</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="381" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" outlineLevel="1">
       <c r="A381" s="6" t="s">
         <v>419</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="382" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:3" outlineLevel="1">
       <c r="A382" s="6" t="s">
         <v>420</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="383" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:3" outlineLevel="1">
       <c r="A383" s="6" t="s">
         <v>421</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="384" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:3" outlineLevel="1">
       <c r="A384" s="6" t="s">
         <v>422</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="385" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:3" outlineLevel="1">
       <c r="A385" s="6" t="s">
         <v>561</v>
       </c>
@@ -7828,19 +7828,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="386" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:3" outlineLevel="1">
       <c r="A386" s="6"/>
       <c r="B386" s="7"/>
       <c r="C386" s="9"/>
     </row>
-    <row r="387" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:3" outlineLevel="1">
       <c r="A387" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B387" s="16"/>
       <c r="C387" s="16"/>
     </row>
-    <row r="388" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:3" ht="28" outlineLevel="1">
       <c r="A388" s="14" t="s">
         <v>699</v>
       </c>
@@ -7851,24 +7851,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="389" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:3" outlineLevel="1">
       <c r="A389" s="14"/>
       <c r="B389" s="7"/>
       <c r="C389" s="9"/>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:3">
       <c r="A390" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B390" s="16"/>
       <c r="C390" s="16"/>
     </row>
-    <row r="391" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" ht="18">
       <c r="A391" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="392" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:3" outlineLevel="1">
       <c r="A392" s="13" t="s">
         <v>460</v>
       </c>
@@ -7879,19 +7879,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="393" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:3" outlineLevel="1">
       <c r="A393" s="13"/>
       <c r="B393" s="5"/>
       <c r="C393" s="9"/>
     </row>
-    <row r="394" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:3" outlineLevel="1">
       <c r="A394" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B394" s="16"/>
       <c r="C394" s="16"/>
     </row>
-    <row r="395" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:3" outlineLevel="1">
       <c r="A395" s="6" t="s">
         <v>461</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="396" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" outlineLevel="1">
       <c r="A396" s="6" t="s">
         <v>462</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:3" ht="56" outlineLevel="1">
       <c r="A397" s="6" t="s">
         <v>463</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" ht="28" outlineLevel="1">
       <c r="A398" s="6" t="s">
         <v>464</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:3" outlineLevel="1">
       <c r="A399" s="6" t="s">
         <v>500</v>
       </c>
@@ -7946,19 +7946,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="400" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:3" outlineLevel="1">
       <c r="A400" s="6"/>
       <c r="B400" s="5"/>
       <c r="C400" s="9"/>
     </row>
-    <row r="401" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:3" outlineLevel="1">
       <c r="A401" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B401" s="16"/>
       <c r="C401" s="16"/>
     </row>
-    <row r="402" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" outlineLevel="1">
       <c r="A402" s="14" t="s">
         <v>465</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:3" outlineLevel="1">
       <c r="A403" s="14" t="s">
         <v>466</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="404" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:3" outlineLevel="1">
       <c r="A404" s="14" t="s">
         <v>467</v>
       </c>
@@ -7991,7 +7991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:3" outlineLevel="1">
       <c r="A405" s="14" t="s">
         <v>468</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="406" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:3" outlineLevel="1">
       <c r="A406" s="14" t="s">
         <v>469</v>
       </c>
@@ -8013,24 +8013,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="407" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:3" outlineLevel="1">
       <c r="A407" s="14"/>
       <c r="B407" s="7"/>
       <c r="C407" s="9"/>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:3">
       <c r="A408" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B408" s="16"/>
       <c r="C408" s="16"/>
     </row>
-    <row r="409" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:3" ht="18">
       <c r="A409" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="410" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:3" outlineLevel="1">
       <c r="A410" s="13" t="s">
         <v>733</v>
       </c>
@@ -8041,19 +8041,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="411" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:3" outlineLevel="1">
       <c r="A411" s="6"/>
       <c r="B411" s="7"/>
       <c r="C411" s="9"/>
     </row>
-    <row r="412" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:3" outlineLevel="1">
       <c r="A412" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B412" s="16"/>
       <c r="C412" s="16"/>
     </row>
-    <row r="413" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:3" outlineLevel="1">
       <c r="A413" s="6" t="s">
         <v>470</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="414" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" outlineLevel="1">
       <c r="A414" s="6" t="s">
         <v>471</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="415" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:3" outlineLevel="1">
       <c r="A415" s="6" t="s">
         <v>472</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="416" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:3" outlineLevel="1">
       <c r="A416" s="6" t="s">
         <v>617</v>
       </c>
@@ -8097,19 +8097,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="417" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:3" outlineLevel="1">
       <c r="A417" s="6"/>
       <c r="B417" s="7"/>
       <c r="C417" s="9"/>
     </row>
-    <row r="418" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:3" outlineLevel="1">
       <c r="A418" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B418" s="16"/>
       <c r="C418" s="16"/>
     </row>
-    <row r="419" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:3" outlineLevel="1">
       <c r="A419" s="14" t="s">
         <v>473</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:3" ht="42" outlineLevel="1">
       <c r="A420" s="14" t="s">
         <v>633</v>
       </c>
@@ -8131,24 +8131,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="421" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:3" outlineLevel="1">
       <c r="A421" s="14"/>
       <c r="B421" s="7"/>
       <c r="C421" s="9"/>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:3">
       <c r="A422" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B422" s="16"/>
       <c r="C422" s="16"/>
     </row>
-    <row r="423" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:3" ht="18">
       <c r="A423" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="424" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:3" outlineLevel="1">
       <c r="A424" s="13" t="s">
         <v>474</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="425" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:3" outlineLevel="1">
       <c r="A425" s="13" t="s">
         <v>475</v>
       </c>
@@ -8170,7 +8170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="426" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:3" outlineLevel="1">
       <c r="A426" s="13" t="s">
         <v>476</v>
       </c>
@@ -8181,19 +8181,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="427" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:3" outlineLevel="1">
       <c r="A427" s="6"/>
       <c r="B427" s="7"/>
       <c r="C427" s="9"/>
     </row>
-    <row r="428" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:3" outlineLevel="1">
       <c r="A428" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B428" s="16"/>
       <c r="C428" s="16"/>
     </row>
-    <row r="429" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:3" outlineLevel="1">
       <c r="A429" s="6" t="s">
         <v>445</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:3" ht="42" outlineLevel="1">
       <c r="A430" s="6" t="s">
         <v>446</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="431" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:3" outlineLevel="1">
       <c r="A431" s="6" t="s">
         <v>447</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="432" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:3" outlineLevel="1">
       <c r="A432" s="6" t="s">
         <v>448</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="433" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:3" outlineLevel="1">
       <c r="A433" s="6" t="s">
         <v>449</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="434" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:3" outlineLevel="1">
       <c r="A434" s="6" t="s">
         <v>450</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:3" outlineLevel="1">
       <c r="A435" s="6" t="s">
         <v>477</v>
       </c>
@@ -8270,19 +8270,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="436" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:3" outlineLevel="1">
       <c r="A436" s="6"/>
       <c r="B436" s="7"/>
       <c r="C436" s="9"/>
     </row>
-    <row r="437" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:3" outlineLevel="1">
       <c r="A437" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B437" s="16"/>
       <c r="C437" s="16"/>
     </row>
-    <row r="438" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:3" outlineLevel="1">
       <c r="A438" s="14" t="s">
         <v>433</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:3" ht="28" outlineLevel="1">
       <c r="A439" s="14" t="s">
         <v>434</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:3" outlineLevel="1">
       <c r="A440" s="14" t="s">
         <v>435</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="441" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:3" outlineLevel="1">
       <c r="A441" s="14" t="s">
         <v>436</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="442" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:3" ht="28" outlineLevel="1">
       <c r="A442" s="14" t="s">
         <v>437</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:3" outlineLevel="1">
       <c r="A443" s="14" t="s">
         <v>438</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="444" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:3" outlineLevel="1">
       <c r="A444" s="14" t="s">
         <v>439</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:3" ht="28" outlineLevel="1">
       <c r="A445" s="14" t="s">
         <v>440</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:3" ht="28" outlineLevel="1">
       <c r="A446" s="14" t="s">
         <v>441</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="447" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:3" outlineLevel="1">
       <c r="A447" s="14" t="s">
         <v>442</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="448" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:3" outlineLevel="1">
       <c r="A448" s="14" t="s">
         <v>443</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:3" outlineLevel="1">
       <c r="A449" s="14" t="s">
         <v>444</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="450" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:3" outlineLevel="1">
       <c r="A450" s="14" t="s">
         <v>504</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="451" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:3" outlineLevel="1">
       <c r="A451" s="14" t="s">
         <v>523</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="452" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:3" outlineLevel="1">
       <c r="A452" s="14" t="s">
         <v>635</v>
       </c>
@@ -8447,24 +8447,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="453" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:3" outlineLevel="1">
       <c r="A453" s="6"/>
       <c r="B453" s="7"/>
       <c r="C453" s="9"/>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:3">
       <c r="A454" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B454" s="16"/>
       <c r="C454" s="16"/>
     </row>
-    <row r="455" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:3" ht="18">
       <c r="A455" s="11" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="456" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:3" outlineLevel="1">
       <c r="A456" s="13" t="s">
         <v>432</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:3" ht="28" outlineLevel="1">
       <c r="A457" s="13" t="s">
         <v>726</v>
       </c>
@@ -8486,19 +8486,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="458" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:3" outlineLevel="1">
       <c r="A458" s="13"/>
       <c r="B458" s="7"/>
       <c r="C458" s="9"/>
     </row>
-    <row r="459" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A459" s="17" t="s">
+    <row r="459" spans="1:3" outlineLevel="1">
+      <c r="A459" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="B459" s="18"/>
-      <c r="C459" s="18"/>
-    </row>
-    <row r="460" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B459" s="20"/>
+      <c r="C459" s="20"/>
+    </row>
+    <row r="460" spans="1:3" outlineLevel="1">
       <c r="A460" s="6" t="s">
         <v>725</v>
       </c>
@@ -8509,19 +8509,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="461" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:3" outlineLevel="1">
       <c r="A461" s="6"/>
       <c r="B461" s="7"/>
       <c r="C461" s="9"/>
     </row>
-    <row r="462" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A462" s="17" t="s">
+    <row r="462" spans="1:3" outlineLevel="1">
+      <c r="A462" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="B462" s="18"/>
-      <c r="C462" s="18"/>
-    </row>
-    <row r="463" spans="1:3" s="4" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B462" s="20"/>
+      <c r="C462" s="20"/>
+    </row>
+    <row r="463" spans="1:3" s="4" customFormat="1" ht="42" outlineLevel="1">
       <c r="A463" s="14" t="s">
         <v>430</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="464" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:3" outlineLevel="1">
       <c r="A464" s="14" t="s">
         <v>431</v>
       </c>
@@ -8543,24 +8543,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="465" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:3" outlineLevel="1">
       <c r="A465" s="14"/>
       <c r="B465" s="7"/>
       <c r="C465" s="9"/>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:3">
       <c r="A466" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B466" s="16"/>
       <c r="C466" s="16"/>
     </row>
-    <row r="467" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:3" ht="18">
       <c r="A467" s="11" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="468" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:3" outlineLevel="1">
       <c r="A468" s="13" t="s">
         <v>731</v>
       </c>
@@ -8571,7 +8571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="469" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:3" outlineLevel="1">
       <c r="A469" s="13" t="s">
         <v>736</v>
       </c>
@@ -8582,14 +8582,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="470" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:3" outlineLevel="1">
       <c r="A470" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B470" s="16"/>
       <c r="C470" s="16"/>
     </row>
-    <row r="471" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:3" outlineLevel="1">
       <c r="A471" s="6" t="s">
         <v>429</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="472" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:3" outlineLevel="1">
       <c r="A472" s="6" t="s">
         <v>482</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="473" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:3" outlineLevel="1">
       <c r="A473" s="6" t="s">
         <v>565</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="474" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:3" outlineLevel="1">
       <c r="A474" s="6" t="s">
         <v>570</v>
       </c>
@@ -8633,19 +8633,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="475" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:3" outlineLevel="1">
       <c r="A475" s="6"/>
       <c r="B475" s="7"/>
       <c r="C475" s="9"/>
     </row>
-    <row r="476" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:3" outlineLevel="1">
       <c r="A476" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B476" s="16"/>
       <c r="C476" s="16"/>
     </row>
-    <row r="477" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:3" ht="28" outlineLevel="1">
       <c r="A477" s="14" t="s">
         <v>423</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="478" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:3" outlineLevel="1">
       <c r="A478" s="14" t="s">
         <v>424</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="479" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:3" outlineLevel="1">
       <c r="A479" s="14" t="s">
         <v>425</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="480" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:3" ht="42" outlineLevel="1">
       <c r="A480" s="14" t="s">
         <v>426</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="481" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:3" ht="28" outlineLevel="1">
       <c r="A481" s="14" t="s">
         <v>427</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="482" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:3" outlineLevel="1">
       <c r="A482" s="14" t="s">
         <v>428</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="483" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:3" outlineLevel="1">
       <c r="A483" s="14" t="s">
         <v>497</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="484" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:3" ht="28" outlineLevel="1">
       <c r="A484" s="14" t="s">
         <v>499</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="485" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:3" outlineLevel="1">
       <c r="A485" s="14" t="s">
         <v>502</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="486" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:3" outlineLevel="1">
       <c r="A486" s="14" t="s">
         <v>503</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="487" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:3" ht="28" outlineLevel="1">
       <c r="A487" s="14" t="s">
         <v>516</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="488" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:3" ht="28" outlineLevel="1">
       <c r="A488" s="14" t="s">
         <v>592</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="489" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:3" ht="28" outlineLevel="1">
       <c r="A489" s="14" t="s">
         <v>602</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="490" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:3" outlineLevel="1">
       <c r="A490" s="14" t="s">
         <v>639</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="491" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:3" ht="28" outlineLevel="1">
       <c r="A491" s="14" t="s">
         <v>687</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="492" spans="1:3" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:3" ht="28" outlineLevel="1">
       <c r="A492" s="14" t="s">
         <v>714</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="493" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:3" ht="28" outlineLevel="1">
       <c r="A493" s="14" t="s">
         <v>717</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="494" spans="1:3" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:3" ht="28" outlineLevel="1">
       <c r="A494" s="14" t="s">
         <v>720</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="495" spans="1:3" s="4" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:3" s="4" customFormat="1" ht="28" outlineLevel="1">
       <c r="A495" s="14" t="s">
         <v>728</v>
       </c>
@@ -8854,63 +8854,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="496" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:3" outlineLevel="1">
       <c r="A496" s="14"/>
       <c r="B496" s="7"/>
       <c r="C496" s="9"/>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:3">
       <c r="A497" s="15" t="s">
         <v>732</v>
       </c>
       <c r="B497" s="16"/>
       <c r="C497" s="16"/>
     </row>
-    <row r="499" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="500" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="501" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="502" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="503" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="504" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="505" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="506" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="507" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="508" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="509" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="510" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="511" spans="1:3" collapsed="1" x14ac:dyDescent="0.25"/>
+    <row r="499" spans="1:3" hidden="1"/>
+    <row r="500" spans="1:3" hidden="1"/>
+    <row r="501" spans="1:3" hidden="1"/>
+    <row r="502" spans="1:3" hidden="1"/>
+    <row r="503" spans="1:3" hidden="1"/>
+    <row r="504" spans="1:3" hidden="1"/>
+    <row r="505" spans="1:3" hidden="1"/>
+    <row r="506" spans="1:3" hidden="1"/>
+    <row r="507" spans="1:3" hidden="1"/>
+    <row r="508" spans="1:3" hidden="1"/>
+    <row r="509" spans="1:3" hidden="1"/>
+    <row r="510" spans="1:3" hidden="1"/>
+    <row r="511" spans="1:3" collapsed="1"/>
   </sheetData>
   <sortState ref="B429:B435">
     <sortCondition ref="B429"/>
   </sortState>
   <mergeCells count="52">
-    <mergeCell ref="A157:C157"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="A146:C146"/>
-    <mergeCell ref="A143:C143"/>
-    <mergeCell ref="A130:C130"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A152:C152"/>
-    <mergeCell ref="A294:C294"/>
-    <mergeCell ref="A289:C289"/>
-    <mergeCell ref="A285:C285"/>
-    <mergeCell ref="A258:C258"/>
-    <mergeCell ref="A262:C262"/>
-    <mergeCell ref="A242:C242"/>
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A237:C237"/>
-    <mergeCell ref="A219:C219"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A204:C204"/>
-    <mergeCell ref="A181:C181"/>
-    <mergeCell ref="A175:C175"/>
-    <mergeCell ref="A165:C165"/>
+    <mergeCell ref="A412:C412"/>
+    <mergeCell ref="A476:C476"/>
+    <mergeCell ref="A470:C470"/>
+    <mergeCell ref="A466:C466"/>
+    <mergeCell ref="A462:C462"/>
+    <mergeCell ref="A459:C459"/>
+    <mergeCell ref="A437:C437"/>
+    <mergeCell ref="A428:C428"/>
+    <mergeCell ref="A454:C454"/>
     <mergeCell ref="A497:C497"/>
     <mergeCell ref="A422:C422"/>
     <mergeCell ref="A418:C418"/>
@@ -8927,15 +8909,33 @@
     <mergeCell ref="A317:C317"/>
     <mergeCell ref="A320:C320"/>
     <mergeCell ref="A347:C347"/>
-    <mergeCell ref="A412:C412"/>
-    <mergeCell ref="A476:C476"/>
-    <mergeCell ref="A470:C470"/>
-    <mergeCell ref="A466:C466"/>
-    <mergeCell ref="A462:C462"/>
-    <mergeCell ref="A459:C459"/>
-    <mergeCell ref="A437:C437"/>
-    <mergeCell ref="A428:C428"/>
-    <mergeCell ref="A454:C454"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A204:C204"/>
+    <mergeCell ref="A181:C181"/>
+    <mergeCell ref="A175:C175"/>
+    <mergeCell ref="A165:C165"/>
+    <mergeCell ref="A242:C242"/>
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A219:C219"/>
+    <mergeCell ref="A294:C294"/>
+    <mergeCell ref="A289:C289"/>
+    <mergeCell ref="A285:C285"/>
+    <mergeCell ref="A258:C258"/>
+    <mergeCell ref="A262:C262"/>
+    <mergeCell ref="A157:C157"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A146:C146"/>
+    <mergeCell ref="A143:C143"/>
+    <mergeCell ref="A130:C130"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A152:C152"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <conditionalFormatting sqref="C205:C211 C471:C475 C463:C465 C460:C461 C377:C386 C455:C458 C498:C1048576 C423:C427 C419:C421 C413:C417 C409 C402:C407 C395:C400 C375 C391:C393 C388:C389 C213:C218 C322 C371 C354:C355 C318:C319 C348:C352 C313:C316 C295:C311 C290:C293 C286:C288 C259:C261 C243:C244 C246:C249 C251:C257 C166:C174 C158:C164 C153:C156 C147:C151 C144:C145 C127 C37:C39 C33:C35 C131:C142 C76:C125 C41:C74 C477:C495 C176:C180 C182:C202 C220:C236 C238:C241 C263:C284 C346 C324 C326 C328 C330 C332 C334 C336 C338 C340 C342 C344 C357:C369 C429:C436 C438:C453 C1:C24 C26:C31 C467:C469">
     <cfRule type="cellIs" dxfId="71" priority="83" operator="equal">
@@ -9168,6 +9168,11 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>